<commit_message>
Release Candidate:before Site check
</commit_message>
<xml_diff>
--- a/BlockGrouping.xlsx
+++ b/BlockGrouping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="640" windowWidth="27980" windowHeight="22100" tabRatio="500"/>
+    <workbookView xWindow="2700" yWindow="680" windowWidth="33360" windowHeight="22420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" workbookViewId="0">
-      <selection sqref="A1:XFD58"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -834,7 +834,7 @@
     </row>
     <row r="34" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G34" t="s">
         <v>27</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="35" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G35" t="s">
         <v>28</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="36" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
         <v>29</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="37" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F37" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
         <v>30</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="38" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G38" t="s">
         <v>31</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="39" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F39" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G39" t="s">
         <v>32</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="40" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F40" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G40" t="s">
         <v>33</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="41" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F41" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G41" t="s">
         <v>34</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="42" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F42" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G42" t="s">
         <v>35</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="43" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F43" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G43" t="s">
         <v>36</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="44" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G44" t="s">
         <v>37</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="45" spans="4:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="F45" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G45" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Strobe color : independent
</commit_message>
<xml_diff>
--- a/BlockGrouping.xlsx
+++ b/BlockGrouping.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="196">
   <si>
     <t>BLOCK_GROUP BlockGrouping[] = {</t>
     <phoneticPr fontId="1"/>
@@ -688,34 +688,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>// b_ColorSync</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>BP_STROBE_24</t>
   </si>
   <si>
@@ -794,16 +766,25 @@
     <t>23,</t>
   </si>
   <si>
-    <t>false</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>"CAM_STROBE_SINGLE_COLOR"</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>"CAM_STROBE_COLOR_SYNC"</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// f_ColorBar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>F_COLORBAR_SYNC</t>
+  </si>
+  <si>
+    <t>F_COLORBAR_COL0</t>
+  </si>
+  <si>
+    <t>F_COLORBAR_STROBE</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1130,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H871"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C791" sqref="C791"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1157,7 +1140,7 @@
     <col min="2" max="2" width="2.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.5703125" bestFit="1" customWidth="1"/>
@@ -1355,13 +1338,13 @@
     </row>
     <row r="21" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E21" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F21" t="s">
         <v>164</v>
       </c>
       <c r="G21" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1615,13 +1598,13 @@
     </row>
     <row r="49" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E49" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F49" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G49" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1809,13 +1792,13 @@
     </row>
     <row r="71" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E71" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F71" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G71" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2003,13 +1986,13 @@
     </row>
     <row r="93" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E93" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F93" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G93" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2263,13 +2246,13 @@
     </row>
     <row r="121" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E121" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F121" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G121" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="122" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2523,13 +2506,13 @@
     </row>
     <row r="149" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E149" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F149" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G149" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="150" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2717,13 +2700,13 @@
     </row>
     <row r="171" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E171" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F171" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G171" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="172" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -2911,13 +2894,13 @@
     </row>
     <row r="193" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E193" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F193" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G193" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="194" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3171,13 +3154,13 @@
     </row>
     <row r="221" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E221" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F221" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G221" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="222" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3224,13 +3207,13 @@
     </row>
     <row r="228" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E228" s="5" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="F228" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G228" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="229" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3484,13 +3467,13 @@
     </row>
     <row r="256" spans="5:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E256" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F256" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G256" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="257" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3537,13 +3520,13 @@
     </row>
     <row r="263" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E263" s="5" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="F263" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G263" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="264" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3797,13 +3780,13 @@
     </row>
     <row r="291" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E291" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F291" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G291" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="292" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3850,13 +3833,13 @@
     </row>
     <row r="298" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E298" s="5" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="F298" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G298" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="299" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4110,13 +4093,13 @@
     </row>
     <row r="326" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E326" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F326" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G326" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="327" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4163,13 +4146,13 @@
     </row>
     <row r="333" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E333" s="5" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="F333" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G333" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="334" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4423,13 +4406,13 @@
     </row>
     <row r="361" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E361" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F361" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G361" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="362" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4683,13 +4666,13 @@
     </row>
     <row r="389" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E389" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F389" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G389" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="390" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -4877,13 +4860,13 @@
     </row>
     <row r="411" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E411" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F411" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G411" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="412" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5071,13 +5054,13 @@
     </row>
     <row r="433" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E433" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F433" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G433" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="434" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5331,13 +5314,13 @@
     </row>
     <row r="461" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E461" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F461" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G461" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="462" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5591,13 +5574,13 @@
     </row>
     <row r="489" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E489" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F489" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G489" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="490" spans="3:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5785,13 +5768,13 @@
     </row>
     <row r="511" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E511" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F511" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G511" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="512" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5979,13 +5962,13 @@
     </row>
     <row r="533" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E533" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F533" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G533" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="534" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6239,13 +6222,13 @@
     </row>
     <row r="561" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E561" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F561" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G561" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="562" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6292,13 +6275,13 @@
     </row>
     <row r="568" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E568" s="5" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="F568" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G568" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="569" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6552,13 +6535,13 @@
     </row>
     <row r="596" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E596" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F596" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G596" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="597" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6605,13 +6588,13 @@
     </row>
     <row r="603" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E603" s="5" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="F603" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G603" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="604" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6865,13 +6848,13 @@
     </row>
     <row r="631" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E631" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F631" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G631" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="632" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -6918,13 +6901,13 @@
     </row>
     <row r="638" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E638" s="5" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="F638" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G638" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="639" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7178,13 +7161,13 @@
     </row>
     <row r="666" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E666" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F666" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G666" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="667" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7231,13 +7214,13 @@
     </row>
     <row r="673" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E673" s="5" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="F673" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G673" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="674" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7370,13 +7353,13 @@
     </row>
     <row r="690" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E690" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F690" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G690" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="691" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7520,13 +7503,13 @@
     </row>
     <row r="708" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E708" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F708" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G708" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="709" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7670,13 +7653,13 @@
     </row>
     <row r="726" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E726" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F726" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G726" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="727" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7820,13 +7803,13 @@
     </row>
     <row r="744" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E744" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F744" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G744" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="745" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7970,13 +7953,13 @@
     </row>
     <row r="762" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E762" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F762" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G762" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="763" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -8120,13 +8103,13 @@
     </row>
     <row r="780" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E780" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F780" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G780" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="781" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -8198,7 +8181,7 @@
         <v>2</v>
       </c>
       <c r="C789" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D789" t="s">
         <v>3</v>
@@ -8206,7 +8189,7 @@
     </row>
     <row r="790" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C790">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D790" t="s">
         <v>3</v>
@@ -8235,7 +8218,7 @@
         <v>2</v>
       </c>
       <c r="G794" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H794" t="s">
         <v>5</v>
@@ -8246,7 +8229,7 @@
         <v>2</v>
       </c>
       <c r="G795" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H795" t="s">
         <v>5</v>
@@ -8257,7 +8240,7 @@
         <v>2</v>
       </c>
       <c r="G796" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="H796" t="s">
         <v>5</v>
@@ -8268,7 +8251,7 @@
         <v>2</v>
       </c>
       <c r="G797" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H797" t="s">
         <v>5</v>
@@ -8279,7 +8262,7 @@
         <v>2</v>
       </c>
       <c r="G798" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H798" t="s">
         <v>5</v>
@@ -8290,7 +8273,7 @@
         <v>2</v>
       </c>
       <c r="G799" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H799" t="s">
         <v>5</v>
@@ -8301,7 +8284,7 @@
         <v>2</v>
       </c>
       <c r="G800" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H800" t="s">
         <v>5</v>
@@ -8312,7 +8295,7 @@
         <v>2</v>
       </c>
       <c r="G801" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H801" t="s">
         <v>5</v>
@@ -8323,7 +8306,7 @@
         <v>2</v>
       </c>
       <c r="G802" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H802" t="s">
         <v>5</v>
@@ -8334,7 +8317,7 @@
         <v>2</v>
       </c>
       <c r="G803" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H803" t="s">
         <v>5</v>
@@ -8345,7 +8328,7 @@
         <v>2</v>
       </c>
       <c r="G804" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H804" t="s">
         <v>5</v>
@@ -8356,7 +8339,7 @@
         <v>2</v>
       </c>
       <c r="G805" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H805" t="s">
         <v>5</v>
@@ -8367,7 +8350,7 @@
         <v>2</v>
       </c>
       <c r="G806" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H806" t="s">
         <v>5</v>
@@ -8378,7 +8361,7 @@
         <v>2</v>
       </c>
       <c r="G807" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="H807" t="s">
         <v>5</v>
@@ -8389,7 +8372,7 @@
         <v>2</v>
       </c>
       <c r="G808" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="H808" t="s">
         <v>5</v>
@@ -8400,7 +8383,7 @@
         <v>2</v>
       </c>
       <c r="G809" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H809" t="s">
         <v>5</v>
@@ -8411,7 +8394,7 @@
         <v>2</v>
       </c>
       <c r="G810" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H810" t="s">
         <v>5</v>
@@ -8422,7 +8405,7 @@
         <v>2</v>
       </c>
       <c r="G811" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H811" t="s">
         <v>5</v>
@@ -8433,7 +8416,7 @@
         <v>2</v>
       </c>
       <c r="G812" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H812" t="s">
         <v>5</v>
@@ -8444,7 +8427,7 @@
         <v>2</v>
       </c>
       <c r="G813" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H813" t="s">
         <v>5</v>
@@ -8455,7 +8438,7 @@
         <v>2</v>
       </c>
       <c r="G814" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="H814" t="s">
         <v>5</v>
@@ -8466,7 +8449,7 @@
         <v>2</v>
       </c>
       <c r="G815" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H815" t="s">
         <v>5</v>
@@ -8477,7 +8460,7 @@
         <v>2</v>
       </c>
       <c r="G816" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H816" t="s">
         <v>5</v>
@@ -8488,7 +8471,7 @@
         <v>2</v>
       </c>
       <c r="G817" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H817" t="s">
         <v>5</v>
@@ -8501,7 +8484,7 @@
     </row>
     <row r="819" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E819" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F819" t="s">
         <v>3</v>
@@ -8512,13 +8495,13 @@
     </row>
     <row r="820" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E820" s="5" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="F820" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G820" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="821" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -8590,7 +8573,7 @@
         <v>2</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D829" t="s">
         <v>3</v>
@@ -8627,7 +8610,7 @@
         <v>2</v>
       </c>
       <c r="G834" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H834" t="s">
         <v>5</v>
@@ -8638,7 +8621,7 @@
         <v>2</v>
       </c>
       <c r="G835" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H835" t="s">
         <v>5</v>
@@ -8649,7 +8632,7 @@
         <v>2</v>
       </c>
       <c r="G836" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="H836" t="s">
         <v>5</v>
@@ -8660,7 +8643,7 @@
         <v>2</v>
       </c>
       <c r="G837" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H837" t="s">
         <v>5</v>
@@ -8671,7 +8654,7 @@
         <v>2</v>
       </c>
       <c r="G838" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H838" t="s">
         <v>5</v>
@@ -8682,7 +8665,7 @@
         <v>2</v>
       </c>
       <c r="G839" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H839" t="s">
         <v>5</v>
@@ -8693,7 +8676,7 @@
         <v>2</v>
       </c>
       <c r="G840" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H840" t="s">
         <v>5</v>
@@ -8704,7 +8687,7 @@
         <v>2</v>
       </c>
       <c r="G841" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H841" t="s">
         <v>5</v>
@@ -8715,7 +8698,7 @@
         <v>2</v>
       </c>
       <c r="G842" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H842" t="s">
         <v>5</v>
@@ -8726,7 +8709,7 @@
         <v>2</v>
       </c>
       <c r="G843" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H843" t="s">
         <v>5</v>
@@ -8737,7 +8720,7 @@
         <v>2</v>
       </c>
       <c r="G844" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H844" t="s">
         <v>5</v>
@@ -8748,7 +8731,7 @@
         <v>2</v>
       </c>
       <c r="G845" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H845" t="s">
         <v>5</v>
@@ -8759,7 +8742,7 @@
         <v>2</v>
       </c>
       <c r="G846" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H846" t="s">
         <v>5</v>
@@ -8770,7 +8753,7 @@
         <v>2</v>
       </c>
       <c r="G847" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="H847" t="s">
         <v>5</v>
@@ -8781,7 +8764,7 @@
         <v>2</v>
       </c>
       <c r="G848" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="H848" t="s">
         <v>5</v>
@@ -8792,7 +8775,7 @@
         <v>2</v>
       </c>
       <c r="G849" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H849" t="s">
         <v>5</v>
@@ -8803,7 +8786,7 @@
         <v>2</v>
       </c>
       <c r="G850" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H850" t="s">
         <v>5</v>
@@ -8814,7 +8797,7 @@
         <v>2</v>
       </c>
       <c r="G851" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H851" t="s">
         <v>5</v>
@@ -8825,7 +8808,7 @@
         <v>2</v>
       </c>
       <c r="G852" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H852" t="s">
         <v>5</v>
@@ -8836,7 +8819,7 @@
         <v>2</v>
       </c>
       <c r="G853" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H853" t="s">
         <v>5</v>
@@ -8847,7 +8830,7 @@
         <v>2</v>
       </c>
       <c r="G854" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="H854" t="s">
         <v>5</v>
@@ -8858,7 +8841,7 @@
         <v>2</v>
       </c>
       <c r="G855" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H855" t="s">
         <v>5</v>
@@ -8869,7 +8852,7 @@
         <v>2</v>
       </c>
       <c r="G856" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H856" t="s">
         <v>5</v>
@@ -8880,7 +8863,7 @@
         <v>2</v>
       </c>
       <c r="G857" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H857" t="s">
         <v>5</v>
@@ -8893,7 +8876,7 @@
     </row>
     <row r="859" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E859" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F859" t="s">
         <v>3</v>
@@ -8904,13 +8887,13 @@
     </row>
     <row r="860" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="E860" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F860" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="G860" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="861" spans="4:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">

</xml_diff>